<commit_message>
party vessels catch. Minor corrections to some xlsx tables
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/Table22.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/Table22.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/fb170/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb170/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07137DE-1D92-3C4B-AB4D-0940F7852596}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4A2509-A2FD-1947-8B3A-7DC8899BB149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19060" yWindow="4500" windowWidth="25320" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -462,7 +472,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -626,7 +636,7 @@
         <v>4583</v>
       </c>
       <c r="E5" s="2">
-        <v>6472</v>
+        <v>6372</v>
       </c>
       <c r="F5" s="2">
         <v>4611</v>
@@ -661,7 +671,7 @@
         <v>27634</v>
       </c>
       <c r="E6" s="2">
-        <v>29368</v>
+        <v>29968</v>
       </c>
       <c r="F6" s="2">
         <v>10598</v>
@@ -1151,7 +1161,7 @@
         <v>5725575</v>
       </c>
       <c r="E20" s="2">
-        <v>5630335</v>
+        <v>5630835</v>
       </c>
       <c r="F20" s="2">
         <v>4604152</v>

</xml_diff>